<commit_message>
jaxine's initial repo update
</commit_message>
<xml_diff>
--- a/personnel_nes-lter-nutrient-transect.xlsx
+++ b/personnel_nes-lter-nutrient-transect.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stace\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-nutrient-transect/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD8C3D5-57AD-A443-B634-ED9C89A2857A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16935"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +57,6 @@
     <t>fundingNumber</t>
   </si>
   <si>
-    <t>PI</t>
-  </si>
-  <si>
     <t>creator</t>
   </si>
   <si>
@@ -101,13 +99,16 @@
     <t>OCE-1655686</t>
   </si>
   <si>
-    <t>Technician</t>
+    <t>principal investigator</t>
+  </si>
+  <si>
+    <t>technician</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,19 +420,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="19.85546875" customWidth="1"/>
+    <col min="1" max="10" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,87 +464,87 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>